<commit_message>
dialogue, task 추가 중
</commit_message>
<xml_diff>
--- a/Excel2Json/bin/haha.xlsx
+++ b/Excel2Json/bin/haha.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Slanted_Structure\Excel2Json\bin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Slanted_Structure\Excel2Json\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C569983B-0425-4595-B4D0-80B1121D02EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBEEBF4-0941-473E-A560-90854FAB5779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a4" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -53,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -144,6 +142,18 @@
   </si>
   <si>
     <t>2번 대화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>asd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>asdasd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaa</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -211,10 +221,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -579,6 +585,34 @@
       </c>
       <c r="D6" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -652,32 +686,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A2F0CC-3FE8-4B20-9350-1D261AAE2A6C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A255231-95F4-47C9-966F-89039C7C7F19}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>